<commit_message>
Initial version of excel generation for grades qualifications
</commit_message>
<xml_diff>
--- a/web/Calificaciones.xlsx
+++ b/web/Calificaciones.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16828"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\expediente\web\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\expediente\web\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9885"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8115"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,8 @@
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Carné</t>
   </si>
@@ -40,12 +41,18 @@
   <si>
     <t>Promedio Trimestral</t>
   </si>
+  <si>
+    <t>Periodo:
+Grupo:
+Materia:
+Profesor:</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -78,6 +85,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -115,7 +129,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -130,118 +144,6 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -259,22 +161,20 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
+      <left/>
+      <right/>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -287,69 +187,68 @@
   </cellStyleXfs>
   <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -479,6 +378,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -514,6 +430,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -666,81 +599,90 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="B1:M7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" customWidth="1"/>
-    <col min="2" max="2" width="38.28515625" customWidth="1"/>
-    <col min="4" max="6" width="8" customWidth="1"/>
+    <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="3" max="3" width="38.28515625" customWidth="1"/>
+    <col min="5" max="7" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="3"/>
-      <c r="B1" s="4"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="8"/>
+    <row r="1" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="7"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="15"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="15"/>
     </row>
-    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="25"/>
+    <row r="2" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="6"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D3" s="13"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="15"/>
+    <row r="3" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E3" s="10"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="12"/>
     </row>
-    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="19" t="s">
+    <row r="4" spans="2:13" s="24" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+    </row>
+    <row r="5" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="17"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:6" ht="183" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="12"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
+    <row r="6" spans="2:13" ht="183" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="17"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B7" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="D7" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="A5:A6"/>
+  <mergeCells count="2">
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="B4:D4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>